<commit_message>
Nasar - 18Nov changes
</commit_message>
<xml_diff>
--- a/src/test/resources/object-repository/OneCSAppiOS.xlsx
+++ b/src/test/resources/object-repository/OneCSAppiOS.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C7D60D-A7DC-A44D-89DE-0A0B2978AEFE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C95CFC4-797D-0D4F-8E86-43CF2842BE5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28680" windowHeight="15920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28680" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iOS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="144">
   <si>
     <t>ELEMENT_KEY</t>
   </si>
@@ -371,6 +371,96 @@
   </si>
   <si>
     <t>sign-in-verify-pin-button</t>
+  </si>
+  <si>
+    <t>Forgot sign in details? Not to worry. Just tap the relevant button below to fix this.</t>
+  </si>
+  <si>
+    <t>FORGOT_SIGN_IN_DETAILS_LABEL_TXT</t>
+  </si>
+  <si>
+    <t>Forgot username</t>
+  </si>
+  <si>
+    <t>FORGOT_USER_NAME_BTN</t>
+  </si>
+  <si>
+    <t>Forgot password</t>
+  </si>
+  <si>
+    <t>FORGOT_PWD_BTN</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>CANCEL_BTN</t>
+  </si>
+  <si>
+    <t>Accept All</t>
+  </si>
+  <si>
+    <t>ACCEPT_ALL_WEBSITE_BTN</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeTextField[@value='YYYY']</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeTextField[@value='DD']</t>
+  </si>
+  <si>
+    <t>DD_FIELD_IN_WEBSITE</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeTextField[@value='MM']</t>
+  </si>
+  <si>
+    <t>MM_FIELD_IN_WEBSITE</t>
+  </si>
+  <si>
+    <t>YYYY_FIELD_IN_WEBSITE</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeOther[@name="Forgotten Username"])[1]/XCUIElementTypeTextField[4]</t>
+  </si>
+  <si>
+    <t>ACCOUNT_NUMBER_FIELD_IN_WEBSITE</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@name='Date Of Birth']</t>
+  </si>
+  <si>
+    <t>DOB_STATIC_TEXT_IN_WEBSITE</t>
+  </si>
+  <si>
+    <t>ACCOUNT_NUMBER_STATIC_TEXT_IN_WEBSITE</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@name='Account Number']</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@name='Forgotten Password']</t>
+  </si>
+  <si>
+    <t>FORGOTTEN_PWD_TXT_IN_WEBSITE</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@name='Username']</t>
+  </si>
+  <si>
+    <t>USERNAME_TXT_IN_WEBSITE</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeButton[@name='Next']</t>
+  </si>
+  <si>
+    <t>NEXT_BTN_IN_WEBSITE</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@name='Forgotten Username']</t>
+  </si>
+  <si>
+    <t>FORGOTTEN_USERNAME_TXT_IN_WEBSITE</t>
   </si>
 </sst>
 </file>
@@ -745,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1382,6 +1472,171 @@
         <v>8</v>
       </c>
     </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57" t="s">
+        <v>114</v>
+      </c>
+      <c r="E57" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" t="s">
+        <v>116</v>
+      </c>
+      <c r="E58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" t="s">
+        <v>118</v>
+      </c>
+      <c r="E59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>121</v>
+      </c>
+      <c r="B60" t="s">
+        <v>120</v>
+      </c>
+      <c r="E60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>123</v>
+      </c>
+      <c r="B61" t="s">
+        <v>122</v>
+      </c>
+      <c r="E61" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>126</v>
+      </c>
+      <c r="B62" t="s">
+        <v>125</v>
+      </c>
+      <c r="E62" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>128</v>
+      </c>
+      <c r="B63" t="s">
+        <v>127</v>
+      </c>
+      <c r="E63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>129</v>
+      </c>
+      <c r="B64" t="s">
+        <v>124</v>
+      </c>
+      <c r="E64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>131</v>
+      </c>
+      <c r="B65" t="s">
+        <v>130</v>
+      </c>
+      <c r="E65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>133</v>
+      </c>
+      <c r="B66" t="s">
+        <v>132</v>
+      </c>
+      <c r="E66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" t="s">
+        <v>135</v>
+      </c>
+      <c r="E67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>137</v>
+      </c>
+      <c r="B68" t="s">
+        <v>136</v>
+      </c>
+      <c r="E68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>139</v>
+      </c>
+      <c r="B69" t="s">
+        <v>138</v>
+      </c>
+      <c r="E69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>141</v>
+      </c>
+      <c r="B70" t="s">
+        <v>140</v>
+      </c>
+      <c r="E70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>143</v>
+      </c>
+      <c r="B71" t="s">
+        <v>142</v>
+      </c>
+      <c r="E71" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Nasar - Nov22 changes
</commit_message>
<xml_diff>
--- a/src/test/resources/object-repository/OneCSAppiOS.xlsx
+++ b/src/test/resources/object-repository/OneCSAppiOS.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1512C1-74E9-F946-90C8-0FE544736F19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8151C906-0729-3140-9802-595A14946303}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28680" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28680" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iOS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="178">
   <si>
     <t>ELEMENT_KEY</t>
   </si>
@@ -545,6 +545,24 @@
   </si>
   <si>
     <t>MEMERABLE_WORD_WEB_TXT</t>
+  </si>
+  <si>
+    <t>SIGN_IN_STEP_4_OF_4_TITLE</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@name="Sign in step 4 of 4"]</t>
+  </si>
+  <si>
+    <t>Create your PIN</t>
+  </si>
+  <si>
+    <t>CREATE_YOUR_PIN_LABEL_TXT</t>
+  </si>
+  <si>
+    <t>You’ll use this 6-digit PIN to log in to your OneCS account securely if you don’t enable Biometrics.</t>
+  </si>
+  <si>
+    <t>YOU_WILL_USE_THIS_PIN_TXT_IN_SIGN3_SCREEN</t>
   </si>
 </sst>
 </file>
@@ -919,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1875,6 +1893,39 @@
         <v>5</v>
       </c>
     </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>172</v>
+      </c>
+      <c r="B86" t="s">
+        <v>173</v>
+      </c>
+      <c r="E86" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>175</v>
+      </c>
+      <c r="B87" t="s">
+        <v>174</v>
+      </c>
+      <c r="E87" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>177</v>
+      </c>
+      <c r="B88" t="s">
+        <v>176</v>
+      </c>
+      <c r="E88" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Nasar - 24th Nov
</commit_message>
<xml_diff>
--- a/src/test/resources/object-repository/OneCSAppiOS.xlsx
+++ b/src/test/resources/object-repository/OneCSAppiOS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85FADFC-2509-6044-9E96-6E79AC72085B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76469AA6-E6D1-A944-ACA6-F3419936C03C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28680" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="199">
   <si>
     <t>ELEMENT_KEY</t>
   </si>
@@ -608,6 +608,24 @@
   </si>
   <si>
     <t>SORRY_PIN_DOES_NOT_MATCH_POP_UP_TXT</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@name="Biometrics disabled"]</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@name="Please go to device setting to enable."]</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>BTN_OK_IN_POP_UP</t>
+  </si>
+  <si>
+    <t>BIOMETRICS_DISABLED_LABEL_TXT</t>
+  </si>
+  <si>
+    <t>PLEASE_GO_TO_DEVICE_SETTINGS_BIO_TXT</t>
   </si>
 </sst>
 </file>
@@ -982,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="G94" sqref="G94"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2059,6 +2077,39 @@
         <v>8</v>
       </c>
     </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>197</v>
+      </c>
+      <c r="B97" t="s">
+        <v>193</v>
+      </c>
+      <c r="E97" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>198</v>
+      </c>
+      <c r="B98" t="s">
+        <v>194</v>
+      </c>
+      <c r="E98" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>196</v>
+      </c>
+      <c r="B99" t="s">
+        <v>195</v>
+      </c>
+      <c r="E99" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Nasar - 1st Dec
</commit_message>
<xml_diff>
--- a/src/test/resources/object-repository/OneCSAppiOS.xlsx
+++ b/src/test/resources/object-repository/OneCSAppiOS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76469AA6-E6D1-A944-ACA6-F3419936C03C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7ACB07D-E631-7E4D-B388-630837108F55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28680" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="321">
   <si>
     <t>ELEMENT_KEY</t>
   </si>
@@ -626,6 +626,372 @@
   </si>
   <si>
     <t>PLEASE_GO_TO_DEVICE_SETTINGS_BIO_TXT</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@name="USER SETTINGS"]</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@name="HELP &amp; SUPPORT"]</t>
+  </si>
+  <si>
+    <t>USER_SETTINGS_LABEL_TXT_MORE</t>
+  </si>
+  <si>
+    <t>HELP_&amp;_SUPPORT_LABEL_TXT_MORE</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@name="MARKETS INFORMATION"]</t>
+  </si>
+  <si>
+    <t>MARKETS_INFORMATION_LABEL_TXT_MORE</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@name="ABOUT CHARLES STANLEY"]</t>
+  </si>
+  <si>
+    <t>ABOUT_CHARLES_STANLEY_LABEL_TXT_MORE</t>
+  </si>
+  <si>
+    <t>Account settings</t>
+  </si>
+  <si>
+    <t>Documents</t>
+  </si>
+  <si>
+    <t>ACCOUNT_SETTINGS_LABEL_TXT_MORE</t>
+  </si>
+  <si>
+    <t>DOCUMENTS_LABEL_TXT_MORE</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeButton[@name="chevron"])[1]</t>
+  </si>
+  <si>
+    <t>ACCOUNT_SETTINGS_CHEVRON</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeButton[@name="chevron"])[2]</t>
+  </si>
+  <si>
+    <t>DOCUMENTS_CHEVRON</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeImage[@name="ic_profile"])[1]</t>
+  </si>
+  <si>
+    <t>ACCOUNT_SETTINGS_PROFILE_IMAGE</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeImage[@name="ic_documents"]</t>
+  </si>
+  <si>
+    <t>DOCUMENTS_IMAGE</t>
+  </si>
+  <si>
+    <t>FAQs</t>
+  </si>
+  <si>
+    <t>FAQS_LABEL_TXT_MORE</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeButton[@name="chevron"])[3]</t>
+  </si>
+  <si>
+    <t>FAQS_CHEVRON</t>
+  </si>
+  <si>
+    <t>ic_faq</t>
+  </si>
+  <si>
+    <t>FAQS_IMAGE</t>
+  </si>
+  <si>
+    <t>Help centre</t>
+  </si>
+  <si>
+    <t>HELP_CENTRE_LABEL_MORE</t>
+  </si>
+  <si>
+    <t>ic_help</t>
+  </si>
+  <si>
+    <t>HELP_IMAGE</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeButton[@name="chevron"])[4]</t>
+  </si>
+  <si>
+    <t>HELP_CHEVRON</t>
+  </si>
+  <si>
+    <t>Glossary</t>
+  </si>
+  <si>
+    <t>GLOSSARY_LABEL_MORE</t>
+  </si>
+  <si>
+    <t>ic_glossary</t>
+  </si>
+  <si>
+    <t>GLOSSARY_IMAGE</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeButton[@name="chevron"])[5]</t>
+  </si>
+  <si>
+    <t>GLOSSARY_CHEVRON</t>
+  </si>
+  <si>
+    <t>What's new</t>
+  </si>
+  <si>
+    <t>WHATS_NEW_LABEL_MORE</t>
+  </si>
+  <si>
+    <t>WHATS_NEW_IMAGE</t>
+  </si>
+  <si>
+    <t>WHATS_NEW_CHEVRON</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeImage[@name="ic_profile"])[2]</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeButton[@name="chevron"])[6]</t>
+  </si>
+  <si>
+    <t>Market data</t>
+  </si>
+  <si>
+    <t>MARKET_DATA_LABEL_MORE</t>
+  </si>
+  <si>
+    <t>MARKET_DATA_IMAGE</t>
+  </si>
+  <si>
+    <t>MARKET_DATA_CHEVRON</t>
+  </si>
+  <si>
+    <t>ic_market_data</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeButton[@name="chevron"])[7]</t>
+  </si>
+  <si>
+    <t>Currency rates</t>
+  </si>
+  <si>
+    <t>CURRENCY_RATES_LABEL_MORE</t>
+  </si>
+  <si>
+    <t>CURRENCY_RATES_IMAGE</t>
+  </si>
+  <si>
+    <t>CURRENCY_RATES_CHEVRON</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeButton[@name="chevron"])[8]</t>
+  </si>
+  <si>
+    <t>ic_currency_rates</t>
+  </si>
+  <si>
+    <t>Contact details</t>
+  </si>
+  <si>
+    <t>CONTACT_DETAILS_LABEL_MORE</t>
+  </si>
+  <si>
+    <t>CONTACT_DETAILS_IMAGE</t>
+  </si>
+  <si>
+    <t>CONTACT_DETAILS_CHEVRON</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeImage[@name="ic_profile"])[3]</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeButton[@name="chevron"])[9]</t>
+  </si>
+  <si>
+    <t>Important information</t>
+  </si>
+  <si>
+    <t>IMPORTANT_INFORMATION_LABEL_MORE</t>
+  </si>
+  <si>
+    <t>IMPORTANT_INFORMATION_IMAGE</t>
+  </si>
+  <si>
+    <t>IMPORTANT_INFORMATION_CHEVRON</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeImage[@name="ic_profile"])[4]</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeButton[@name="chevron"])[10]</t>
+  </si>
+  <si>
+    <t>Licensing information</t>
+  </si>
+  <si>
+    <t>LICENSING_INFORMATION_LABEL_MORE</t>
+  </si>
+  <si>
+    <t>LICENSING_INFORMATION_IMAGE</t>
+  </si>
+  <si>
+    <t>LICENSING_INFORMATION_CHEVRON</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeImage[@name="ic_profile"])[5]</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeButton[@name="chevron"])[11]</t>
+  </si>
+  <si>
+    <t>Rate us</t>
+  </si>
+  <si>
+    <t>RATE_US_LABEL_MORE</t>
+  </si>
+  <si>
+    <t>RATE_US_LABEL_IMAGE</t>
+  </si>
+  <si>
+    <t>RATE_US_LABEL_CHEVRON</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeImage[@name="ic_profile"])[6]</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeButton[@name="chevron"])[12]</t>
+  </si>
+  <si>
+    <t>portfolio-account-0-name</t>
+  </si>
+  <si>
+    <t>PORTFOLIO_ACCOUNT_NAME_YOUR_ACCOUNTS_1</t>
+  </si>
+  <si>
+    <t>select-account-button</t>
+  </si>
+  <si>
+    <t>ACCOUNT_DASHBOARD_SELECT_ACCOUNT_BTN</t>
+  </si>
+  <si>
+    <t>ic account management</t>
+  </si>
+  <si>
+    <t>ACCOUNT_MANAGEMENT_PENCIL_BTN</t>
+  </si>
+  <si>
+    <t>account-summary-name</t>
+  </si>
+  <si>
+    <t>ACCOUNT_SUMMARY_NAME_LABEL_TXT</t>
+  </si>
+  <si>
+    <t>Your account value is</t>
+  </si>
+  <si>
+    <t>YOUR_ACCOUNT_VALUE_IS_LABEL_TXT</t>
+  </si>
+  <si>
+    <t>account-performance-increase-arrow</t>
+  </si>
+  <si>
+    <t>ACCOUNT_PERFORMANCE_INCREASE_ARROW</t>
+  </si>
+  <si>
+    <t>account-summary-total-value</t>
+  </si>
+  <si>
+    <t>ACCOUNT_SUMMARY_TOTAL_VALUE_LABEL</t>
+  </si>
+  <si>
+    <t>account-summary-value-change</t>
+  </si>
+  <si>
+    <t>ACCOUNT_SUMMARY_VALUE_CHANGE_LABEL</t>
+  </si>
+  <si>
+    <t>account-summary-refreshed-at-text</t>
+  </si>
+  <si>
+    <t>ACCOUNT_SUMMARY_REFRESH_AT_LABEL</t>
+  </si>
+  <si>
+    <t>account-toggle-values-button</t>
+  </si>
+  <si>
+    <t>EYE_SIGN_IN_ACCOUNT_DASHBOARD_BTN</t>
+  </si>
+  <si>
+    <t>Holdings</t>
+  </si>
+  <si>
+    <t>HOLDINGS_DRAG_UP_BTN</t>
+  </si>
+  <si>
+    <t>account-close-management-button</t>
+  </si>
+  <si>
+    <t>ACCOUNT_MANAGEMENT_CLOSE_BTN</t>
+  </si>
+  <si>
+    <t>Account management</t>
+  </si>
+  <si>
+    <t>ACCOUNT_MANAGEMENT_DRAG_UP_BTN</t>
+  </si>
+  <si>
+    <t>ACCOUNT_ACTIVITY_BTN</t>
+  </si>
+  <si>
+    <t>ACCOUNT_BREAKDOWN_BTN</t>
+  </si>
+  <si>
+    <t>Account breakdown</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Order list</t>
+  </si>
+  <si>
+    <t>ORDER_LIST_TAB</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@name="Account activity"]</t>
+  </si>
+  <si>
+    <t>ACCOUNT_ACTIVITY_SCREEN_LABEL_TXT</t>
+  </si>
+  <si>
+    <t>account-activity-0-type</t>
+  </si>
+  <si>
+    <t>ACCOUNT_ACTIVITY_1ST_ACTIVITY_NAME_TXT</t>
+  </si>
+  <si>
+    <t>account-activity-0-icon</t>
+  </si>
+  <si>
+    <t>ACCOUNT_ACTIVITY_1ST_ACTIVITY_ICON_TXT</t>
+  </si>
+  <si>
+    <t>account-activity-0-value</t>
+  </si>
+  <si>
+    <t>ACCOUNT_ACTIVITY_1ST_ACTIVITY_VALUE_TXT</t>
+  </si>
+  <si>
+    <t>account-activity-0-transaction-type</t>
+  </si>
+  <si>
+    <t>ACCOUNT_ACTIVITY_1ST_ACTIVITY_TRANSACTION_TYPE_TXT</t>
   </si>
 </sst>
 </file>
@@ -1000,15 +1366,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="84.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
@@ -2110,6 +2476,682 @@
         <v>8</v>
       </c>
     </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>201</v>
+      </c>
+      <c r="B100" t="s">
+        <v>199</v>
+      </c>
+      <c r="E100" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>202</v>
+      </c>
+      <c r="B101" t="s">
+        <v>200</v>
+      </c>
+      <c r="E101" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>204</v>
+      </c>
+      <c r="B102" t="s">
+        <v>203</v>
+      </c>
+      <c r="E102" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>206</v>
+      </c>
+      <c r="B103" t="s">
+        <v>205</v>
+      </c>
+      <c r="E103" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>209</v>
+      </c>
+      <c r="B104" t="s">
+        <v>207</v>
+      </c>
+      <c r="E104" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>210</v>
+      </c>
+      <c r="B105" t="s">
+        <v>208</v>
+      </c>
+      <c r="E105" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>212</v>
+      </c>
+      <c r="B106" t="s">
+        <v>211</v>
+      </c>
+      <c r="E106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>214</v>
+      </c>
+      <c r="B107" t="s">
+        <v>213</v>
+      </c>
+      <c r="E107" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>216</v>
+      </c>
+      <c r="B108" t="s">
+        <v>215</v>
+      </c>
+      <c r="E108" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>218</v>
+      </c>
+      <c r="B109" t="s">
+        <v>217</v>
+      </c>
+      <c r="E109" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>220</v>
+      </c>
+      <c r="B110" t="s">
+        <v>219</v>
+      </c>
+      <c r="E110" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>222</v>
+      </c>
+      <c r="B111" t="s">
+        <v>221</v>
+      </c>
+      <c r="E111" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>224</v>
+      </c>
+      <c r="B112" t="s">
+        <v>223</v>
+      </c>
+      <c r="E112" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>226</v>
+      </c>
+      <c r="B113" t="s">
+        <v>225</v>
+      </c>
+      <c r="E113" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>228</v>
+      </c>
+      <c r="B114" t="s">
+        <v>227</v>
+      </c>
+      <c r="E114" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>230</v>
+      </c>
+      <c r="B115" t="s">
+        <v>229</v>
+      </c>
+      <c r="E115" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>232</v>
+      </c>
+      <c r="B116" t="s">
+        <v>231</v>
+      </c>
+      <c r="E116" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>234</v>
+      </c>
+      <c r="B117" t="s">
+        <v>233</v>
+      </c>
+      <c r="E117" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>236</v>
+      </c>
+      <c r="B118" t="s">
+        <v>235</v>
+      </c>
+      <c r="E118" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>238</v>
+      </c>
+      <c r="B119" t="s">
+        <v>237</v>
+      </c>
+      <c r="E119" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>239</v>
+      </c>
+      <c r="B120" t="s">
+        <v>241</v>
+      </c>
+      <c r="E120" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>240</v>
+      </c>
+      <c r="B121" t="s">
+        <v>242</v>
+      </c>
+      <c r="E121" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>244</v>
+      </c>
+      <c r="B122" t="s">
+        <v>243</v>
+      </c>
+      <c r="E122" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>245</v>
+      </c>
+      <c r="B123" t="s">
+        <v>247</v>
+      </c>
+      <c r="E123" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>246</v>
+      </c>
+      <c r="B124" t="s">
+        <v>248</v>
+      </c>
+      <c r="E124" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>250</v>
+      </c>
+      <c r="B125" t="s">
+        <v>249</v>
+      </c>
+      <c r="E125" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>251</v>
+      </c>
+      <c r="B126" t="s">
+        <v>254</v>
+      </c>
+      <c r="E126" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>252</v>
+      </c>
+      <c r="B127" t="s">
+        <v>253</v>
+      </c>
+      <c r="E127" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>256</v>
+      </c>
+      <c r="B128" t="s">
+        <v>255</v>
+      </c>
+      <c r="E128" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>257</v>
+      </c>
+      <c r="B129" t="s">
+        <v>259</v>
+      </c>
+      <c r="E129" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>258</v>
+      </c>
+      <c r="B130" t="s">
+        <v>260</v>
+      </c>
+      <c r="E130" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>262</v>
+      </c>
+      <c r="B131" t="s">
+        <v>261</v>
+      </c>
+      <c r="E131" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>263</v>
+      </c>
+      <c r="B132" t="s">
+        <v>265</v>
+      </c>
+      <c r="E132" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>264</v>
+      </c>
+      <c r="B133" t="s">
+        <v>266</v>
+      </c>
+      <c r="E133" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>268</v>
+      </c>
+      <c r="B134" t="s">
+        <v>267</v>
+      </c>
+      <c r="E134" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>269</v>
+      </c>
+      <c r="B135" t="s">
+        <v>271</v>
+      </c>
+      <c r="E135" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>270</v>
+      </c>
+      <c r="B136" t="s">
+        <v>272</v>
+      </c>
+      <c r="E136" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>274</v>
+      </c>
+      <c r="B137" t="s">
+        <v>273</v>
+      </c>
+      <c r="E137" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>275</v>
+      </c>
+      <c r="B138" t="s">
+        <v>277</v>
+      </c>
+      <c r="E138" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>276</v>
+      </c>
+      <c r="B139" t="s">
+        <v>278</v>
+      </c>
+      <c r="E139" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>280</v>
+      </c>
+      <c r="B140" t="s">
+        <v>279</v>
+      </c>
+      <c r="E140" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>282</v>
+      </c>
+      <c r="B141" t="s">
+        <v>281</v>
+      </c>
+      <c r="E141" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>284</v>
+      </c>
+      <c r="B142" t="s">
+        <v>283</v>
+      </c>
+      <c r="E142" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>286</v>
+      </c>
+      <c r="B143" t="s">
+        <v>285</v>
+      </c>
+      <c r="E143" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>288</v>
+      </c>
+      <c r="B144" t="s">
+        <v>287</v>
+      </c>
+      <c r="E144" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>290</v>
+      </c>
+      <c r="B145" t="s">
+        <v>289</v>
+      </c>
+      <c r="E145" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>292</v>
+      </c>
+      <c r="B146" t="s">
+        <v>291</v>
+      </c>
+      <c r="E146" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>294</v>
+      </c>
+      <c r="B147" t="s">
+        <v>293</v>
+      </c>
+      <c r="E147" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>296</v>
+      </c>
+      <c r="B148" t="s">
+        <v>295</v>
+      </c>
+      <c r="E148" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>298</v>
+      </c>
+      <c r="B149" t="s">
+        <v>297</v>
+      </c>
+      <c r="E149" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>300</v>
+      </c>
+      <c r="B150" t="s">
+        <v>299</v>
+      </c>
+      <c r="E150" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>302</v>
+      </c>
+      <c r="B151" t="s">
+        <v>301</v>
+      </c>
+      <c r="E151" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>304</v>
+      </c>
+      <c r="B152" t="s">
+        <v>303</v>
+      </c>
+      <c r="E152" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>305</v>
+      </c>
+      <c r="B153" t="s">
+        <v>308</v>
+      </c>
+      <c r="E153" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>306</v>
+      </c>
+      <c r="B154" t="s">
+        <v>307</v>
+      </c>
+      <c r="E154" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>310</v>
+      </c>
+      <c r="B155" t="s">
+        <v>309</v>
+      </c>
+      <c r="E155" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>312</v>
+      </c>
+      <c r="B156" t="s">
+        <v>311</v>
+      </c>
+      <c r="E156" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>314</v>
+      </c>
+      <c r="B157" t="s">
+        <v>313</v>
+      </c>
+      <c r="E157" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>316</v>
+      </c>
+      <c r="B158" t="s">
+        <v>315</v>
+      </c>
+      <c r="E158" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>318</v>
+      </c>
+      <c r="B159" t="s">
+        <v>317</v>
+      </c>
+      <c r="E159" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>320</v>
+      </c>
+      <c r="B160" t="s">
+        <v>319</v>
+      </c>
+      <c r="E160" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="161" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E161" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Nasar - 27th Dec
</commit_message>
<xml_diff>
--- a/src/test/resources/object-repository/OneCSAppiOS.xlsx
+++ b/src/test/resources/object-repository/OneCSAppiOS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D7C893-4D9D-374B-8965-D40341F5CDFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36682015-E9E1-B142-8BBD-3962A599A5A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28680" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="453">
   <si>
     <t>ELEMENT_KEY</t>
   </si>
@@ -952,9 +952,6 @@
     <t>Activity</t>
   </si>
   <si>
-    <t>Order list</t>
-  </si>
-  <si>
     <t>ORDER_LIST_TAB</t>
   </si>
   <si>
@@ -1262,6 +1259,135 @@
   </si>
   <si>
     <t>DASH_SIGN_IN_PORTFOLIO_BREAKDOWN</t>
+  </si>
+  <si>
+    <t>order-list-tab-button</t>
+  </si>
+  <si>
+    <t>activity-tab-button</t>
+  </si>
+  <si>
+    <t>ACTIVITY_TAB</t>
+  </si>
+  <si>
+    <t>Pay money in</t>
+  </si>
+  <si>
+    <t>PAY_MONEY_IN_BTN_ACC_MANAGEMENT</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@label="CANCELLED"]</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@label="COMPLETE"]</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@label="PROCESSING"]</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@label="DEALT"]</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@label="REJECTED"]</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeStaticText[@label="EXPIRED"]</t>
+  </si>
+  <si>
+    <t>ORDER_TYPE_CANCELLED</t>
+  </si>
+  <si>
+    <t>ORDER_TYPE_COMPLETE</t>
+  </si>
+  <si>
+    <t>ORDER_TYPE_PROCESSING</t>
+  </si>
+  <si>
+    <t>ORDER_TYPE_DEALT</t>
+  </si>
+  <si>
+    <t>ORDER_TYPE_REJECTED</t>
+  </si>
+  <si>
+    <t>ORDER_TYPE_EXPIRED</t>
+  </si>
+  <si>
+    <t>close-order-details-button</t>
+  </si>
+  <si>
+    <t>CLOSE_ORDER_DETAILS_BTN</t>
+  </si>
+  <si>
+    <t>Order detail</t>
+  </si>
+  <si>
+    <t>ORDER_DETAILS_TITLE</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ORDER_DETAIL_STATUS_FIELD</t>
+  </si>
+  <si>
+    <t>Trade type</t>
+  </si>
+  <si>
+    <t>ORDER_DETAIL_TRADE_TYPE_FIELD</t>
+  </si>
+  <si>
+    <t>(//XCUIElementTypeStaticText[@name="Date"])[9]</t>
+  </si>
+  <si>
+    <t>ORDER_DETAIL_DATE_FIELD</t>
+  </si>
+  <si>
+    <t>Settlement date</t>
+  </si>
+  <si>
+    <t>ORDER_DETAIL_SETTLEMENT_DATE_FIELD</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>ORDER_DETAIL_PRICE_FIELD</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>ORDER_DETAIL_QUANTITY_FIELD</t>
+  </si>
+  <si>
+    <t>Consideration</t>
+  </si>
+  <si>
+    <t>ORDER_DETAIL_CONSIDERATION_FIELD</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>ORDER_DETAIL_OTHER_FIELD</t>
+  </si>
+  <si>
+    <t>Dealing fee</t>
+  </si>
+  <si>
+    <t>ORDER_DETAIL_DEALING_FEE_FIELD</t>
+  </si>
+  <si>
+    <t>Estimated value</t>
+  </si>
+  <si>
+    <t>ORDER_DETAIL_ESTIMATED_VALUE_FIELD</t>
+  </si>
+  <si>
+    <t>cancel-order-button</t>
+  </si>
+  <si>
+    <t>ORDER_DETAIL_CANCEL_ORDER_BTN</t>
   </si>
 </sst>
 </file>
@@ -1636,10 +1762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E205"/>
+  <dimension ref="A1:E226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="B195" sqref="B195"/>
+    <sheetView tabSelected="1" topLeftCell="A210" workbookViewId="0">
+      <selection activeCell="B229" sqref="B229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1882,7 +2008,7 @@
         <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E21" t="s">
         <v>5</v>
@@ -2044,7 +2170,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B36" t="s">
         <v>69</v>
@@ -3353,10 +3479,10 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B155" t="s">
-        <v>307</v>
+        <v>410</v>
       </c>
       <c r="E155" t="s">
         <v>8</v>
@@ -3364,10 +3490,10 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B156" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E156" t="s">
         <v>5</v>
@@ -3375,10 +3501,10 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B157" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E157" t="s">
         <v>8</v>
@@ -3386,10 +3512,10 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B158" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E158" t="s">
         <v>8</v>
@@ -3397,10 +3523,10 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B159" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E159" t="s">
         <v>8</v>
@@ -3408,10 +3534,10 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B160" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E160" t="s">
         <v>8</v>
@@ -3419,10 +3545,10 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B161" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E161" t="s">
         <v>8</v>
@@ -3430,10 +3556,10 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B162" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E162" t="s">
         <v>5</v>
@@ -3441,10 +3567,10 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B163" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E163" t="s">
         <v>8</v>
@@ -3452,10 +3578,10 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B164" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E164" t="s">
         <v>5</v>
@@ -3463,10 +3589,10 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B165" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E165" t="s">
         <v>5</v>
@@ -3474,10 +3600,10 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B166" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E166" t="s">
         <v>5</v>
@@ -3485,10 +3611,10 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B167" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E167" t="s">
         <v>5</v>
@@ -3496,10 +3622,10 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B168" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E168" t="s">
         <v>8</v>
@@ -3507,10 +3633,10 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B169" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E169" t="s">
         <v>8</v>
@@ -3518,10 +3644,10 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B170" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E170" t="s">
         <v>8</v>
@@ -3529,10 +3655,10 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B171" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E171" t="s">
         <v>8</v>
@@ -3540,10 +3666,10 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B172" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E172" t="s">
         <v>8</v>
@@ -3551,10 +3677,10 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B173" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E173" t="s">
         <v>8</v>
@@ -3562,10 +3688,10 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B174" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E174" t="s">
         <v>5</v>
@@ -3573,10 +3699,10 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B175" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E175" t="s">
         <v>8</v>
@@ -3584,10 +3710,10 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B176" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E176" t="s">
         <v>5</v>
@@ -3595,10 +3721,10 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B177" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E177" t="s">
         <v>5</v>
@@ -3606,10 +3732,10 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B178" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E178" t="s">
         <v>5</v>
@@ -3617,10 +3743,10 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B179" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E179" t="s">
         <v>5</v>
@@ -3628,10 +3754,10 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B180" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E180" t="s">
         <v>8</v>
@@ -3639,10 +3765,10 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B181" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E181" t="s">
         <v>8</v>
@@ -3650,10 +3776,10 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B182" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E182" t="s">
         <v>5</v>
@@ -3661,10 +3787,10 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B183" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E183" t="s">
         <v>8</v>
@@ -3672,10 +3798,10 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B184" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E184" t="s">
         <v>8</v>
@@ -3683,10 +3809,10 @@
     </row>
     <row r="185" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E185" t="s">
         <v>5</v>
@@ -3694,10 +3820,10 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B186" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E186" t="s">
         <v>8</v>
@@ -3705,10 +3831,10 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B187" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E187" t="s">
         <v>8</v>
@@ -3716,10 +3842,10 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B188" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E188" t="s">
         <v>8</v>
@@ -3727,10 +3853,10 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B189" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E189" t="s">
         <v>8</v>
@@ -3738,10 +3864,10 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B190" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E190" t="s">
         <v>5</v>
@@ -3749,10 +3875,10 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B191" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E191" t="s">
         <v>8</v>
@@ -3760,10 +3886,10 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B192" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E192" t="s">
         <v>8</v>
@@ -3771,10 +3897,10 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B193" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E193" t="s">
         <v>8</v>
@@ -3782,10 +3908,10 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B194" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E194" t="s">
         <v>8</v>
@@ -3793,10 +3919,10 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B195" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E195" t="s">
         <v>8</v>
@@ -3804,10 +3930,10 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B196" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E196" t="s">
         <v>8</v>
@@ -3815,10 +3941,10 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B197" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E197" t="s">
         <v>8</v>
@@ -3826,10 +3952,10 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B198" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E198" t="s">
         <v>8</v>
@@ -3837,10 +3963,10 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B199" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E199" t="s">
         <v>5</v>
@@ -3848,10 +3974,10 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B200" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E200" t="s">
         <v>5</v>
@@ -3859,10 +3985,10 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B201" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E201" t="s">
         <v>5</v>
@@ -3870,10 +3996,10 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B202" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E202" t="s">
         <v>5</v>
@@ -3881,10 +4007,10 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B203" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E203" t="s">
         <v>5</v>
@@ -3892,10 +4018,10 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B204" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E204" t="s">
         <v>5</v>
@@ -3903,13 +4029,244 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B205" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E205" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>412</v>
+      </c>
+      <c r="B206" t="s">
+        <v>411</v>
+      </c>
+      <c r="E206" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>414</v>
+      </c>
+      <c r="B207" t="s">
+        <v>413</v>
+      </c>
+      <c r="E207" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>421</v>
+      </c>
+      <c r="B208" t="s">
+        <v>415</v>
+      </c>
+      <c r="E208" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>422</v>
+      </c>
+      <c r="B209" t="s">
+        <v>416</v>
+      </c>
+      <c r="E209" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>423</v>
+      </c>
+      <c r="B210" t="s">
+        <v>417</v>
+      </c>
+      <c r="E210" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>424</v>
+      </c>
+      <c r="B211" t="s">
+        <v>418</v>
+      </c>
+      <c r="E211" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>425</v>
+      </c>
+      <c r="B212" t="s">
+        <v>419</v>
+      </c>
+      <c r="E212" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>426</v>
+      </c>
+      <c r="B213" t="s">
+        <v>420</v>
+      </c>
+      <c r="E213" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>428</v>
+      </c>
+      <c r="B214" t="s">
+        <v>427</v>
+      </c>
+      <c r="E214" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>430</v>
+      </c>
+      <c r="B215" t="s">
+        <v>429</v>
+      </c>
+      <c r="E215" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>432</v>
+      </c>
+      <c r="B216" t="s">
+        <v>431</v>
+      </c>
+      <c r="E216" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>434</v>
+      </c>
+      <c r="B217" t="s">
+        <v>433</v>
+      </c>
+      <c r="E217" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>436</v>
+      </c>
+      <c r="B218" t="s">
+        <v>435</v>
+      </c>
+      <c r="E218" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>438</v>
+      </c>
+      <c r="B219" t="s">
+        <v>437</v>
+      </c>
+      <c r="E219" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>440</v>
+      </c>
+      <c r="B220" t="s">
+        <v>439</v>
+      </c>
+      <c r="E220" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>442</v>
+      </c>
+      <c r="B221" t="s">
+        <v>441</v>
+      </c>
+      <c r="E221" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>444</v>
+      </c>
+      <c r="B222" t="s">
+        <v>443</v>
+      </c>
+      <c r="E222" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>446</v>
+      </c>
+      <c r="B223" t="s">
+        <v>445</v>
+      </c>
+      <c r="E223" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>448</v>
+      </c>
+      <c r="B224" t="s">
+        <v>447</v>
+      </c>
+      <c r="E224" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>450</v>
+      </c>
+      <c r="B225" t="s">
+        <v>449</v>
+      </c>
+      <c r="E225" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>452</v>
+      </c>
+      <c r="B226" t="s">
+        <v>451</v>
+      </c>
+      <c r="E226" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nasar - 28th Dec
</commit_message>
<xml_diff>
--- a/src/test/resources/object-repository/OneCSAppiOS.xlsx
+++ b/src/test/resources/object-repository/OneCSAppiOS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36682015-E9E1-B142-8BBD-3962A599A5A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F95F906-B204-6240-B441-A0827D5ADA26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28680" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="461">
   <si>
     <t>ELEMENT_KEY</t>
   </si>
@@ -1388,6 +1388,30 @@
   </si>
   <si>
     <t>ORDER_DETAIL_CANCEL_ORDER_BTN</t>
+  </si>
+  <si>
+    <t>Select account</t>
+  </si>
+  <si>
+    <t>SELECT_ACCOUNT_TITLE</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>SELECT_ACCOUNT_CLOSE_BTN</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeOther[@name="CURRENTLY SELECTED"]</t>
+  </si>
+  <si>
+    <t>CURRENTLY_SELECTED_LABEL</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeOther[@name="OTHER ACCOUNTS"]</t>
+  </si>
+  <si>
+    <t>OTHER_ACCOUNTS_LABEL</t>
   </si>
 </sst>
 </file>
@@ -1762,10 +1786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E226"/>
+  <dimension ref="A1:E230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" workbookViewId="0">
-      <selection activeCell="B229" sqref="B229"/>
+    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
+      <selection activeCell="B233" sqref="B233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4269,6 +4293,50 @@
         <v>8</v>
       </c>
     </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>454</v>
+      </c>
+      <c r="B227" t="s">
+        <v>453</v>
+      </c>
+      <c r="E227" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>456</v>
+      </c>
+      <c r="B228" t="s">
+        <v>455</v>
+      </c>
+      <c r="E228" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>458</v>
+      </c>
+      <c r="B229" t="s">
+        <v>457</v>
+      </c>
+      <c r="E229" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>460</v>
+      </c>
+      <c r="B230" t="s">
+        <v>459</v>
+      </c>
+      <c r="E230" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>